<commit_message>
[product-importing] Acceptance test for product importing
</commit_message>
<xml_diff>
--- a/app/tests/assets/messed_up_products.xlsx
+++ b/app/tests/assets/messed_up_products.xlsx
@@ -61,9 +61,6 @@
     <t>Descrição de um produto com detalhes</t>
   </si>
   <si>
-    <t>Verde</t>
-  </si>
-  <si>
     <t>Outra coisa valida</t>
   </si>
   <si>
@@ -71,17 +68,26 @@
   </si>
   <si>
     <t>algum valor</t>
+  </si>
+  <si>
+    <t>Não existente</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -173,13 +179,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +548,9 @@
         <v>1</v>
       </c>
       <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
+      <c r="G5" s="5">
+        <v>3</v>
+      </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
     </row>
@@ -564,14 +573,14 @@
         <v>3</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -589,7 +598,7 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5" t="s">
@@ -597,13 +606,14 @@
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
+      <c r="H8" s="6"/>
       <c r="I8" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[product-importing] Acceptance test for record success on importing
</commit_message>
<xml_diff>
--- a/app/tests/assets/messed_up_products.xlsx
+++ b/app/tests/assets/messed_up_products.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Categoria</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>Não existente</t>
+  </si>
+  <si>
+    <t>Coisa Valida</t>
   </si>
 </sst>
 </file>
@@ -490,8 +493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,11 +599,12 @@
       <c r="A8" s="5">
         <v>8800001</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="C8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="5"/>
       <c r="E8" s="5" t="s">
         <v>1</v>
       </c>

</xml_diff>